<commit_message>
added to final cpu, updated instructions
</commit_message>
<xml_diff>
--- a/Instruction_set.xlsx
+++ b/Instruction_set.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="983" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="77">
   <si>
     <t>1 nibble</t>
   </si>
@@ -113,39 +113,45 @@
     <t>a</t>
   </si>
   <si>
+    <t>Imm 1</t>
+  </si>
+  <si>
+    <t>Imm 2</t>
+  </si>
+  <si>
+    <t>load from RAM (imm, imm) </t>
+  </si>
+  <si>
+    <t>Rd=RAM[arg2arg3]</t>
+  </si>
+  <si>
+    <t>1011</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>load from RAM (register) </t>
+  </si>
+  <si>
+    <t>Rd=RAM[Ra]</t>
+  </si>
+  <si>
+    <t>1100</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>start register </t>
+  </si>
+  <si>
     <t>imm(p1)</t>
   </si>
   <si>
     <t>Imm(p2)</t>
   </si>
   <si>
-    <t>load from RAM (imm, imm) </t>
-  </si>
-  <si>
-    <t>Rd=RAM[arg2arg3]</t>
-  </si>
-  <si>
-    <t>1011</t>
-  </si>
-  <si>
-    <t>b</t>
-  </si>
-  <si>
-    <t>load from RAM (register) </t>
-  </si>
-  <si>
-    <t>Rd=RAM[Ra]</t>
-  </si>
-  <si>
-    <t>1100</t>
-  </si>
-  <si>
-    <t>c</t>
-  </si>
-  <si>
-    <t>start register </t>
-  </si>
-  <si>
     <t>store to RAM(imm, imm)</t>
   </si>
   <si>
@@ -158,7 +164,7 @@
     <t>d</t>
   </si>
   <si>
-    <t>imm</t>
+    <t>Imm 3</t>
   </si>
   <si>
     <t>RAM[arg2arg3]=arg1</t>
@@ -182,7 +188,7 @@
     <t>f</t>
   </si>
   <si>
-    <t>compare register to register &amp; goto</t>
+    <t>save imm1imm2 to destination register</t>
   </si>
   <si>
     <t>Cycle tasks:</t>
@@ -434,8 +440,8 @@
   </sheetPr>
   <dimension ref="A1:P89"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D61" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="P93" activeCellId="0" sqref="P93"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F19" activeCellId="0" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -470,6 +476,7 @@
       <c r="E1" s="3" t="s">
         <v>0</v>
       </c>
+      <c r="M1" s="0"/>
       <c r="N1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -491,6 +498,7 @@
       <c r="F2" s="0" t="s">
         <v>6</v>
       </c>
+      <c r="M2" s="0"/>
       <c r="N2" s="0"/>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -512,6 +520,7 @@
       <c r="F3" s="0" t="s">
         <v>11</v>
       </c>
+      <c r="M3" s="0"/>
       <c r="N3" s="0"/>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -533,6 +542,7 @@
       <c r="F4" s="0" t="s">
         <v>13</v>
       </c>
+      <c r="M4" s="0"/>
       <c r="N4" s="0"/>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -554,6 +564,7 @@
       <c r="F5" s="0" t="s">
         <v>15</v>
       </c>
+      <c r="M5" s="0"/>
       <c r="N5" s="0"/>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -575,6 +586,7 @@
       <c r="F6" s="0" t="s">
         <v>17</v>
       </c>
+      <c r="M6" s="0"/>
       <c r="N6" s="0"/>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -596,6 +608,7 @@
       <c r="F7" s="0" t="s">
         <v>19</v>
       </c>
+      <c r="M7" s="0"/>
       <c r="N7" s="0"/>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -617,6 +630,7 @@
       <c r="F8" s="0" t="s">
         <v>21</v>
       </c>
+      <c r="M8" s="0"/>
       <c r="N8" s="0"/>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -638,6 +652,7 @@
       <c r="F9" s="0" t="s">
         <v>23</v>
       </c>
+      <c r="M9" s="0"/>
       <c r="N9" s="0"/>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -659,6 +674,7 @@
       <c r="F10" s="0" t="s">
         <v>25</v>
       </c>
+      <c r="M10" s="0"/>
       <c r="N10" s="0"/>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -680,6 +696,7 @@
       <c r="F11" s="0" t="s">
         <v>27</v>
       </c>
+      <c r="M11" s="0"/>
       <c r="N11" s="0"/>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -701,6 +718,7 @@
       <c r="F12" s="0" t="s">
         <v>29</v>
       </c>
+      <c r="M12" s="0"/>
       <c r="N12" s="0"/>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -725,6 +743,7 @@
       <c r="I13" s="0" t="s">
         <v>35</v>
       </c>
+      <c r="M13" s="0"/>
       <c r="N13" s="0"/>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -747,6 +766,7 @@
       <c r="I14" s="0" t="s">
         <v>39</v>
       </c>
+      <c r="M14" s="0"/>
       <c r="N14" s="0"/>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -760,164 +780,174 @@
         <v>42</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>33</v>
+        <v>44</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="I15" s="0" t="s">
-        <v>44</v>
-      </c>
+        <v>46</v>
+      </c>
+      <c r="M15" s="0"/>
       <c r="N15" s="0"/>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C16" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="D16" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="E16" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="F16" s="0" t="s">
         <v>45</v>
       </c>
-      <c r="B16" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="C16" s="0" t="s">
-        <v>47</v>
-      </c>
-      <c r="D16" s="0" t="s">
-        <v>47</v>
-      </c>
-      <c r="E16" s="0" t="s">
-        <v>47</v>
-      </c>
-      <c r="F16" s="0" t="s">
-        <v>43</v>
-      </c>
       <c r="I16" s="0" t="s">
-        <v>48</v>
-      </c>
+        <v>50</v>
+      </c>
+      <c r="M16" s="0"/>
       <c r="N16" s="0"/>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="4" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C17" s="0" t="s">
         <v>9</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>47</v>
+        <v>32</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="F17" s="0" t="s">
-        <v>52</v>
-      </c>
+        <v>54</v>
+      </c>
+      <c r="M17" s="0"/>
       <c r="N17" s="0"/>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="4" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>10</v>
+        <v>32</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>51</v>
+        <v>33</v>
       </c>
       <c r="F18" s="0" t="s">
-        <v>55</v>
-      </c>
+        <v>57</v>
+      </c>
+      <c r="M18" s="0"/>
       <c r="N18" s="0"/>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0"/>
+      <c r="M19" s="0"/>
       <c r="N19" s="0"/>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0"/>
+      <c r="M20" s="0"/>
       <c r="N20" s="0"/>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0"/>
+      <c r="M21" s="0"/>
       <c r="N21" s="0"/>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0"/>
       <c r="B22" s="3" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="F22" s="0" t="s">
-        <v>60</v>
-      </c>
+        <v>62</v>
+      </c>
+      <c r="M22" s="0"/>
       <c r="N22" s="0"/>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0"/>
+      <c r="M23" s="0"/>
       <c r="N23" s="0"/>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="6" t="s">
-        <v>61</v>
-      </c>
+        <v>63</v>
+      </c>
+      <c r="M24" s="0"/>
       <c r="N24" s="0"/>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0"/>
       <c r="B25" s="0" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="F25" s="0" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="G25" s="0" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="I25" s="0" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="J25" s="0" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="K25" s="0" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="L25" s="0" t="s">
-        <v>71</v>
-      </c>
-      <c r="M25" s="2" t="s">
-        <v>72</v>
+        <v>73</v>
+      </c>
+      <c r="M25" s="7" t="s">
+        <v>74</v>
       </c>
       <c r="N25" s="0"/>
       <c r="P25" s="7" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -954,7 +984,7 @@
       <c r="L26" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="M26" s="2" t="n">
+      <c r="M26" s="7" t="n">
         <v>0</v>
       </c>
       <c r="N26" s="0"/>
@@ -996,12 +1026,12 @@
       <c r="L27" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="M27" s="2" t="n">
+      <c r="M27" s="7" t="n">
         <v>0</v>
       </c>
       <c r="N27" s="0"/>
       <c r="P27" s="7" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1026,6 +1056,7 @@
       <c r="G28" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="M28" s="0"/>
       <c r="N28" s="0"/>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1050,6 +1081,7 @@
       <c r="G29" s="0" t="n">
         <v>1</v>
       </c>
+      <c r="M29" s="0"/>
       <c r="N29" s="0"/>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1086,7 +1118,7 @@
       <c r="L30" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="M30" s="2" t="n">
+      <c r="M30" s="7" t="n">
         <v>0</v>
       </c>
       <c r="N30" s="0"/>
@@ -1128,12 +1160,12 @@
       <c r="L31" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="M31" s="2" t="n">
+      <c r="M31" s="7" t="n">
         <v>0</v>
       </c>
       <c r="N31" s="0"/>
       <c r="P31" s="7" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1158,6 +1190,7 @@
       <c r="G32" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="M32" s="0"/>
       <c r="N32" s="0"/>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1182,6 +1215,7 @@
       <c r="G33" s="0" t="n">
         <v>1</v>
       </c>
+      <c r="M33" s="0"/>
       <c r="N33" s="0"/>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1218,7 +1252,7 @@
       <c r="L34" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="M34" s="2" t="n">
+      <c r="M34" s="7" t="n">
         <v>0</v>
       </c>
       <c r="N34" s="0"/>
@@ -1260,12 +1294,12 @@
       <c r="L35" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="M35" s="2" t="n">
+      <c r="M35" s="7" t="n">
         <v>0</v>
       </c>
       <c r="N35" s="0"/>
       <c r="P35" s="7" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1290,6 +1324,7 @@
       <c r="G36" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="M36" s="0"/>
       <c r="N36" s="0"/>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1314,6 +1349,7 @@
       <c r="G37" s="0" t="n">
         <v>1</v>
       </c>
+      <c r="M37" s="0"/>
       <c r="N37" s="0"/>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1350,7 +1386,7 @@
       <c r="L38" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="M38" s="2" t="n">
+      <c r="M38" s="7" t="n">
         <v>0</v>
       </c>
       <c r="N38" s="0"/>
@@ -1392,12 +1428,12 @@
       <c r="L39" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="M39" s="2" t="n">
+      <c r="M39" s="7" t="n">
         <v>0</v>
       </c>
       <c r="N39" s="0"/>
       <c r="P39" s="7" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1422,6 +1458,7 @@
       <c r="G40" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="M40" s="0"/>
       <c r="N40" s="0"/>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1446,6 +1483,7 @@
       <c r="G41" s="0" t="n">
         <v>1</v>
       </c>
+      <c r="M41" s="0"/>
       <c r="N41" s="0"/>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1482,7 +1520,7 @@
       <c r="L42" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="M42" s="2" t="n">
+      <c r="M42" s="7" t="n">
         <v>0</v>
       </c>
       <c r="N42" s="0"/>
@@ -1524,12 +1562,12 @@
       <c r="L43" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="M43" s="2" t="n">
+      <c r="M43" s="7" t="n">
         <v>0</v>
       </c>
       <c r="N43" s="0"/>
       <c r="P43" s="7" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1554,6 +1592,7 @@
       <c r="G44" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="M44" s="0"/>
       <c r="N44" s="0"/>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1578,6 +1617,7 @@
       <c r="G45" s="0" t="n">
         <v>1</v>
       </c>
+      <c r="M45" s="0"/>
       <c r="N45" s="0"/>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1614,7 +1654,7 @@
       <c r="L46" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="M46" s="2" t="n">
+      <c r="M46" s="7" t="n">
         <v>0</v>
       </c>
       <c r="N46" s="0"/>
@@ -1656,12 +1696,12 @@
       <c r="L47" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="M47" s="2" t="n">
+      <c r="M47" s="7" t="n">
         <v>0</v>
       </c>
       <c r="N47" s="0"/>
       <c r="P47" s="7" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1686,6 +1726,7 @@
       <c r="G48" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="M48" s="0"/>
       <c r="N48" s="0"/>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1710,6 +1751,7 @@
       <c r="G49" s="0" t="n">
         <v>1</v>
       </c>
+      <c r="M49" s="0"/>
       <c r="N49" s="0"/>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1746,7 +1788,7 @@
       <c r="L50" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="M50" s="2" t="n">
+      <c r="M50" s="7" t="n">
         <v>0</v>
       </c>
       <c r="N50" s="0"/>
@@ -1788,12 +1830,12 @@
       <c r="L51" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="M51" s="2" t="n">
+      <c r="M51" s="7" t="n">
         <v>0</v>
       </c>
       <c r="N51" s="0"/>
       <c r="P51" s="7" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1818,6 +1860,7 @@
       <c r="G52" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="M52" s="0"/>
       <c r="N52" s="0"/>
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1842,6 +1885,7 @@
       <c r="G53" s="0" t="n">
         <v>1</v>
       </c>
+      <c r="M53" s="0"/>
       <c r="N53" s="0"/>
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1878,7 +1922,7 @@
       <c r="L54" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="M54" s="2" t="n">
+      <c r="M54" s="7" t="n">
         <v>0</v>
       </c>
       <c r="N54" s="0"/>
@@ -1920,12 +1964,12 @@
       <c r="L55" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="M55" s="2" t="n">
+      <c r="M55" s="7" t="n">
         <v>0</v>
       </c>
       <c r="N55" s="0"/>
       <c r="P55" s="7" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1950,6 +1994,7 @@
       <c r="G56" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="M56" s="0"/>
       <c r="N56" s="0"/>
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1974,6 +2019,7 @@
       <c r="G57" s="0" t="n">
         <v>1</v>
       </c>
+      <c r="M57" s="0"/>
       <c r="N57" s="0"/>
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2010,7 +2056,7 @@
       <c r="L58" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="M58" s="2" t="n">
+      <c r="M58" s="7" t="n">
         <v>0</v>
       </c>
       <c r="N58" s="0"/>
@@ -2052,12 +2098,12 @@
       <c r="L59" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="M59" s="2" t="n">
+      <c r="M59" s="7" t="n">
         <v>0</v>
       </c>
       <c r="N59" s="0"/>
       <c r="P59" s="7" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2082,6 +2128,7 @@
       <c r="G60" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="M60" s="0"/>
       <c r="N60" s="0"/>
     </row>
     <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2106,6 +2153,7 @@
       <c r="G61" s="0" t="n">
         <v>1</v>
       </c>
+      <c r="M61" s="0"/>
       <c r="N61" s="0"/>
     </row>
     <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2142,7 +2190,7 @@
       <c r="L62" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="M62" s="2" t="n">
+      <c r="M62" s="7" t="n">
         <v>0</v>
       </c>
       <c r="N62" s="0"/>
@@ -2184,12 +2232,12 @@
       <c r="L63" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="M63" s="2" t="n">
+      <c r="M63" s="7" t="n">
         <v>0</v>
       </c>
       <c r="N63" s="0"/>
       <c r="P63" s="7" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2214,8 +2262,9 @@
       <c r="G64" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="M64" s="0"/>
       <c r="N64" s="0"/>
-      <c r="P64" s="2"/>
+      <c r="P64" s="7"/>
     </row>
     <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="6" t="n">
@@ -2239,8 +2288,9 @@
       <c r="G65" s="0" t="n">
         <v>1</v>
       </c>
+      <c r="M65" s="0"/>
       <c r="N65" s="0"/>
-      <c r="P65" s="2"/>
+      <c r="P65" s="7"/>
     </row>
     <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="6" t="s">
@@ -2276,11 +2326,11 @@
       <c r="L66" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="M66" s="2" t="n">
+      <c r="M66" s="7" t="n">
         <v>0</v>
       </c>
       <c r="N66" s="0"/>
-      <c r="P66" s="2" t="n">
+      <c r="P66" s="7" t="n">
         <v>20</v>
       </c>
     </row>
@@ -2318,11 +2368,11 @@
       <c r="L67" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="M67" s="2" t="n">
+      <c r="M67" s="7" t="n">
         <v>0</v>
       </c>
       <c r="N67" s="0"/>
-      <c r="P67" s="2" t="n">
+      <c r="P67" s="7" t="n">
         <v>60</v>
       </c>
     </row>
@@ -2348,8 +2398,9 @@
       <c r="G68" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="M68" s="0"/>
       <c r="N68" s="0"/>
-      <c r="P68" s="2"/>
+      <c r="P68" s="7"/>
     </row>
     <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="6" t="s">
@@ -2373,8 +2424,9 @@
       <c r="G69" s="0" t="n">
         <v>1</v>
       </c>
+      <c r="M69" s="0"/>
       <c r="N69" s="0"/>
-      <c r="P69" s="2"/>
+      <c r="P69" s="7"/>
     </row>
     <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="6" t="s">
@@ -2410,11 +2462,11 @@
       <c r="L70" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="M70" s="2" t="n">
+      <c r="M70" s="7" t="n">
         <v>0</v>
       </c>
       <c r="N70" s="0"/>
-      <c r="P70" s="2" t="n">
+      <c r="P70" s="7" t="n">
         <v>20</v>
       </c>
     </row>
@@ -2452,11 +2504,11 @@
       <c r="L71" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="M71" s="2" t="n">
+      <c r="M71" s="7" t="n">
         <v>0</v>
       </c>
       <c r="N71" s="0"/>
-      <c r="P71" s="2" t="n">
+      <c r="P71" s="7" t="n">
         <v>60</v>
       </c>
     </row>
@@ -2482,8 +2534,9 @@
       <c r="G72" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="M72" s="0"/>
       <c r="N72" s="0"/>
-      <c r="P72" s="2"/>
+      <c r="P72" s="7"/>
     </row>
     <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="6" t="s">
@@ -2507,8 +2560,9 @@
       <c r="G73" s="0" t="n">
         <v>1</v>
       </c>
+      <c r="M73" s="0"/>
       <c r="N73" s="0"/>
-      <c r="P73" s="2"/>
+      <c r="P73" s="7"/>
     </row>
     <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="6" t="s">
@@ -2544,11 +2598,11 @@
       <c r="L74" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="M74" s="2" t="n">
+      <c r="M74" s="7" t="n">
         <v>0</v>
       </c>
       <c r="N74" s="0"/>
-      <c r="P74" s="2" t="n">
+      <c r="P74" s="7" t="n">
         <v>80</v>
       </c>
     </row>
@@ -2586,11 +2640,11 @@
       <c r="L75" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="M75" s="2" t="n">
+      <c r="M75" s="7" t="n">
         <v>0</v>
       </c>
       <c r="N75" s="0"/>
-      <c r="P75" s="2" t="n">
+      <c r="P75" s="7" t="n">
         <v>90</v>
       </c>
     </row>
@@ -2616,8 +2670,9 @@
       <c r="G76" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="M76" s="0"/>
       <c r="N76" s="0"/>
-      <c r="P76" s="2"/>
+      <c r="P76" s="7"/>
     </row>
     <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="6" t="s">
@@ -2641,12 +2696,13 @@
       <c r="G77" s="0" t="n">
         <v>1</v>
       </c>
+      <c r="M77" s="0"/>
       <c r="N77" s="0"/>
-      <c r="P77" s="2"/>
+      <c r="P77" s="7"/>
     </row>
     <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="6" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B78" s="0" t="n">
         <v>1</v>
@@ -2678,17 +2734,17 @@
       <c r="L78" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="M78" s="2" t="n">
+      <c r="M78" s="7" t="n">
         <v>0</v>
       </c>
       <c r="N78" s="0"/>
-      <c r="P78" s="2" t="n">
+      <c r="P78" s="7" t="n">
         <v>80</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="6" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B79" s="0" t="n">
         <v>1</v>
@@ -2720,17 +2776,17 @@
       <c r="L79" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="M79" s="2" t="n">
+      <c r="M79" s="7" t="n">
         <v>0</v>
       </c>
       <c r="N79" s="0"/>
-      <c r="P79" s="2" t="n">
+      <c r="P79" s="7" t="n">
         <v>90</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="6" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B80" s="0" t="n">
         <v>1</v>
@@ -2750,12 +2806,13 @@
       <c r="G80" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="M80" s="0"/>
       <c r="N80" s="0"/>
-      <c r="P80" s="2"/>
+      <c r="P80" s="7"/>
     </row>
     <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="6" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B81" s="0" t="n">
         <v>1</v>
@@ -2775,12 +2832,13 @@
       <c r="G81" s="0" t="n">
         <v>1</v>
       </c>
+      <c r="M81" s="0"/>
       <c r="N81" s="0"/>
-      <c r="P81" s="2"/>
+      <c r="P81" s="7"/>
     </row>
     <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="6" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B82" s="0" t="n">
         <v>1</v>
@@ -2812,17 +2870,17 @@
       <c r="L82" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="M82" s="2" t="n">
+      <c r="M82" s="7" t="n">
         <v>0</v>
       </c>
       <c r="N82" s="0"/>
-      <c r="P82" s="2" t="n">
+      <c r="P82" s="7" t="n">
         <v>80</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="6" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B83" s="0" t="n">
         <v>1</v>
@@ -2854,17 +2912,17 @@
       <c r="L83" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="M83" s="2" t="n">
+      <c r="M83" s="7" t="n">
         <v>1</v>
       </c>
       <c r="N83" s="0"/>
-      <c r="P83" s="2" t="n">
+      <c r="P83" s="7" t="n">
         <v>81</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="6" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B84" s="0" t="n">
         <v>1</v>
@@ -2884,12 +2942,13 @@
       <c r="G84" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="M84" s="0"/>
       <c r="N84" s="0"/>
-      <c r="P84" s="2"/>
+      <c r="P84" s="7"/>
     </row>
     <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="6" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B85" s="0" t="n">
         <v>1</v>
@@ -2909,12 +2968,13 @@
       <c r="G85" s="0" t="n">
         <v>1</v>
       </c>
+      <c r="M85" s="0"/>
       <c r="N85" s="0"/>
-      <c r="P85" s="2"/>
+      <c r="P85" s="7"/>
     </row>
     <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="6" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B86" s="0" t="n">
         <v>1</v>
@@ -2946,17 +3006,17 @@
       <c r="L86" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="M86" s="2" t="n">
+      <c r="M86" s="7" t="n">
         <v>0</v>
       </c>
       <c r="N86" s="0"/>
-      <c r="P86" s="2" t="n">
+      <c r="P86" s="7" t="n">
         <v>80</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="6" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B87" s="0" t="n">
         <v>1</v>
@@ -2988,17 +3048,17 @@
       <c r="L87" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="M87" s="2" t="n">
+      <c r="M87" s="7" t="n">
         <v>1</v>
       </c>
       <c r="N87" s="0"/>
-      <c r="P87" s="2" t="n">
+      <c r="P87" s="7" t="n">
         <v>81</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="6" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B88" s="0" t="n">
         <v>1</v>
@@ -3019,11 +3079,11 @@
         <v>0</v>
       </c>
       <c r="N88" s="0"/>
-      <c r="P88" s="2"/>
+      <c r="P88" s="7"/>
     </row>
     <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="6" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B89" s="0" t="n">
         <v>1</v>
@@ -3044,7 +3104,7 @@
         <v>1</v>
       </c>
       <c r="N89" s="0"/>
-      <c r="P89" s="2"/>
+      <c r="P89" s="7"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
tested a few instructions, fixed clock increment by
</commit_message>
<xml_diff>
--- a/Instruction_set.xlsx
+++ b/Instruction_set.xlsx
@@ -15,11 +15,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="92">
   <si>
     <t>1 nibble</t>
   </si>
   <si>
+    <t>Tested and works?</t>
+  </si>
+  <si>
     <t>opcode(binary)</t>
   </si>
   <si>
@@ -56,6 +59,9 @@
     <t>ADD Rd, Ra, Rb</t>
   </si>
   <si>
+    <t>yes</t>
+  </si>
+  <si>
     <t>0001</t>
   </si>
   <si>
@@ -227,6 +233,9 @@
     <t>Rd=arg2arg3</t>
   </si>
   <si>
+    <t>Yes</t>
+  </si>
+  <si>
     <t>Cycle tasks:</t>
   </si>
   <si>
@@ -282,9 +291,6 @@
   </si>
   <si>
     <t>c0</t>
-  </si>
-  <si>
-    <t>8c</t>
   </si>
 </sst>
 </file>
@@ -480,7 +486,7 @@
   <dimension ref="A1:P89"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C18" activeCellId="0" sqref="C18:E18"/>
+      <selection pane="topLeft" activeCell="L5" activeCellId="0" sqref="L5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -515,425 +521,437 @@
       <c r="E1" s="3" t="s">
         <v>0</v>
       </c>
+      <c r="L1" s="0" t="s">
+        <v>1</v>
+      </c>
       <c r="M1" s="0"/>
       <c r="N1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="M2" s="0"/>
       <c r="N2" s="0"/>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B3" s="3" t="n">
         <v>0</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="I3" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
+      </c>
+      <c r="L3" s="0" t="s">
+        <v>14</v>
       </c>
       <c r="M3" s="0"/>
       <c r="N3" s="0"/>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B4" s="3" t="n">
         <v>1</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F4" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="I4" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="L4" s="0" t="s">
         <v>14</v>
-      </c>
-      <c r="I4" s="0" t="s">
-        <v>15</v>
       </c>
       <c r="M4" s="0"/>
       <c r="N4" s="0"/>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="4" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B5" s="3" t="n">
         <v>2</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="I5" s="0" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="M5" s="0"/>
       <c r="N5" s="0"/>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="4" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B6" s="3" t="n">
         <v>3</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="I6" s="0" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="M6" s="0"/>
       <c r="N6" s="0"/>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="4" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B7" s="3" t="n">
         <v>4</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="I7" s="0" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="M7" s="0"/>
       <c r="N7" s="0"/>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="4" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B8" s="3" t="n">
         <v>5</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="I8" s="0" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="M8" s="0"/>
       <c r="N8" s="0"/>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="4" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B9" s="3" t="n">
         <v>6</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="I9" s="0" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="M9" s="0"/>
       <c r="N9" s="0"/>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="4" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B10" s="3" t="n">
         <v>7</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="I10" s="0" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="M10" s="0"/>
       <c r="N10" s="0"/>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="4" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B11" s="3" t="n">
         <v>8</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="I11" s="0" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="M11" s="0"/>
       <c r="N11" s="0"/>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="4" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B12" s="3" t="n">
         <v>9</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="I12" s="0" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="M12" s="0"/>
       <c r="N12" s="0"/>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="4" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="I13" s="0" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="M13" s="0"/>
       <c r="N13" s="0"/>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="4" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E14" s="5"/>
       <c r="F14" s="0" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="I14" s="0" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="M14" s="0"/>
       <c r="N14" s="0"/>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="4" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="I15" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="M15" s="0"/>
       <c r="N15" s="0"/>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C16" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="D16" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="E16" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="F16" s="0" t="s">
         <v>56</v>
       </c>
-      <c r="B16" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="C16" s="0" t="s">
-        <v>58</v>
-      </c>
-      <c r="D16" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="E16" s="0" t="s">
-        <v>43</v>
-      </c>
-      <c r="F16" s="0" t="s">
-        <v>54</v>
-      </c>
       <c r="I16" s="0" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="M16" s="0"/>
       <c r="N16" s="0"/>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="4" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="F17" s="0" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="I17" s="0" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="M17" s="0"/>
       <c r="N17" s="0"/>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="4" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="F18" s="0" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="I18" s="0" t="s">
-        <v>69</v>
+        <v>71</v>
+      </c>
+      <c r="L18" s="0" t="s">
+        <v>72</v>
       </c>
       <c r="M18" s="0"/>
       <c r="N18" s="0"/>
@@ -956,19 +974,19 @@
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0"/>
       <c r="B22" s="3" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="F22" s="0" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="M22" s="0"/>
       <c r="N22" s="0"/>
@@ -980,7 +998,7 @@
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="6" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="M24" s="0"/>
       <c r="N24" s="0"/>
@@ -988,41 +1006,41 @@
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0"/>
       <c r="B25" s="0" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="F25" s="0" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="G25" s="0" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="I25" s="0" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="J25" s="0" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="K25" s="0" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="L25" s="0" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="M25" s="7" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="N25" s="0"/>
       <c r="P25" s="7" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1106,7 +1124,7 @@
       </c>
       <c r="N27" s="0"/>
       <c r="P27" s="7" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1240,7 +1258,7 @@
       </c>
       <c r="N31" s="0"/>
       <c r="P31" s="7" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1374,7 +1392,7 @@
       </c>
       <c r="N35" s="0"/>
       <c r="P35" s="7" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1508,7 +1526,7 @@
       </c>
       <c r="N39" s="0"/>
       <c r="P39" s="7" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1642,7 +1660,7 @@
       </c>
       <c r="N43" s="0"/>
       <c r="P43" s="7" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1776,7 +1794,7 @@
       </c>
       <c r="N47" s="0"/>
       <c r="P47" s="7" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1910,7 +1928,7 @@
       </c>
       <c r="N51" s="0"/>
       <c r="P51" s="7" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2044,7 +2062,7 @@
       </c>
       <c r="N55" s="0"/>
       <c r="P55" s="7" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2178,7 +2196,7 @@
       </c>
       <c r="N59" s="0"/>
       <c r="P59" s="7" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2312,7 +2330,7 @@
       </c>
       <c r="N63" s="0"/>
       <c r="P63" s="7" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2369,7 +2387,7 @@
     </row>
     <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="6" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B66" s="0" t="n">
         <v>1</v>
@@ -2411,7 +2429,7 @@
     </row>
     <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="6" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B67" s="0" t="n">
         <v>1</v>
@@ -2453,7 +2471,7 @@
     </row>
     <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="6" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B68" s="0" t="n">
         <v>1</v>
@@ -2479,7 +2497,7 @@
     </row>
     <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="6" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B69" s="0" t="n">
         <v>1</v>
@@ -2505,7 +2523,7 @@
     </row>
     <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="6" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B70" s="0" t="n">
         <v>1</v>
@@ -2547,7 +2565,7 @@
     </row>
     <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="6" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B71" s="0" t="n">
         <v>1</v>
@@ -2589,7 +2607,7 @@
     </row>
     <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="6" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B72" s="0" t="n">
         <v>1</v>
@@ -2615,7 +2633,7 @@
     </row>
     <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="6" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B73" s="0" t="n">
         <v>1</v>
@@ -2641,7 +2659,7 @@
     </row>
     <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="6" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B74" s="0" t="n">
         <v>1</v>
@@ -2683,7 +2701,7 @@
     </row>
     <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="6" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B75" s="0" t="n">
         <v>1</v>
@@ -2725,7 +2743,7 @@
     </row>
     <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="6" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B76" s="0" t="n">
         <v>1</v>
@@ -2751,7 +2769,7 @@
     </row>
     <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="6" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B77" s="0" t="n">
         <v>1</v>
@@ -2777,7 +2795,7 @@
     </row>
     <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="6" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B78" s="0" t="n">
         <v>1</v>
@@ -2819,7 +2837,7 @@
     </row>
     <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="6" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B79" s="0" t="n">
         <v>1</v>
@@ -2861,7 +2879,7 @@
     </row>
     <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="6" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B80" s="0" t="n">
         <v>1</v>
@@ -2887,7 +2905,7 @@
     </row>
     <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="6" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B81" s="0" t="n">
         <v>1</v>
@@ -2913,7 +2931,7 @@
     </row>
     <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="6" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="B82" s="0" t="n">
         <v>1</v>
@@ -2955,7 +2973,7 @@
     </row>
     <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="6" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="B83" s="0" t="n">
         <v>1</v>
@@ -2997,7 +3015,7 @@
     </row>
     <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="6" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="B84" s="0" t="n">
         <v>1</v>
@@ -3023,7 +3041,7 @@
     </row>
     <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="6" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="B85" s="0" t="n">
         <v>1</v>
@@ -3049,7 +3067,7 @@
     </row>
     <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="6" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B86" s="0" t="n">
         <v>1</v>
@@ -3091,7 +3109,7 @@
     </row>
     <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="6" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B87" s="0" t="n">
         <v>1</v>
@@ -3128,12 +3146,12 @@
       </c>
       <c r="N87" s="0"/>
       <c r="P87" s="7" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="6" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B88" s="0" t="n">
         <v>1</v>
@@ -3158,7 +3176,7 @@
     </row>
     <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="6" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B89" s="0" t="n">
         <v>1</v>

</xml_diff>